<commit_message>
repo clean-up, jochen's slides
</commit_message>
<xml_diff>
--- a/RapidMiner/classification_results/Evaluation_latex.xlsx
+++ b/RapidMiner/classification_results/Evaluation_latex.xlsx
@@ -117,7 +117,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>SVM</c:v>
+            <c:v>SVM (Acc.: 50.0%)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -201,7 +201,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Naive Bayes</c:v>
+            <c:v>Naive Bayes (Acc.: 50%)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -252,6 +252,10 @@
               </c:spPr>
             </c:marker>
           </c:dPt>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$D$10:$E$10</c:f>
@@ -287,7 +291,7 @@
           <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>50-NN Basic</c:v>
+            <c:v>50-NN Basic (Acc.: 81.3%)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -344,6 +348,21 @@
               </c:spPr>
             </c:marker>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.4436548925328883E-2"/>
+                  <c:y val="-3.864734299516908E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$F$10:$G$10</c:f>
@@ -379,7 +398,7 @@
           <c:idx val="6"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>50-NN Weighted</c:v>
+            <c:v>50-NN Weighted (Acc.: 75.0%)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -437,6 +456,10 @@
               </c:spPr>
             </c:marker>
           </c:dPt>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$H$10:$I$10</c:f>
@@ -468,11 +491,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73144192"/>
-        <c:axId val="73142272"/>
+        <c:axId val="95293824"/>
+        <c:axId val="95296128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73144192"/>
+        <c:axId val="95293824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,12 +520,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73142272"/>
+        <c:crossAx val="95296128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73142272"/>
+        <c:axId val="95296128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +551,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73144192"/>
+        <c:crossAx val="95293824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -541,7 +564,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -869,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>